<commit_message>
Alterações feitas a task 3 adicionei mais componentes
</commit_message>
<xml_diff>
--- a/front-end/Task 3.xlsx
+++ b/front-end/Task 3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40F649-D66E-4727-9D1A-32CADC0A580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7968ADE4-81EF-4F56-BFF9-429A184DCC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Views</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Talvez tenha?</t>
-  </si>
-  <si>
     <t>Highlights</t>
   </si>
   <si>
@@ -117,12 +114,6 @@
     <t>See more</t>
   </si>
   <si>
-    <t>Não é suposto fazer me thinks</t>
-  </si>
-  <si>
-    <t>Meat?</t>
-  </si>
-  <si>
     <t>Year bar</t>
   </si>
   <si>
@@ -142,6 +133,18 @@
   </si>
   <si>
     <t>Slider</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Top bar</t>
+  </si>
+  <si>
+    <t>Top Bar + Header</t>
   </si>
 </sst>
 </file>
@@ -243,12 +246,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -260,26 +284,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -303,15 +321,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>396673</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>131779</xdr:rowOff>
+      <xdr:colOff>247586</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1092327</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>388650</xdr:rowOff>
+      <xdr:colOff>1234109</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>413172</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -339,8 +357,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2621468" y="2172960"/>
-          <a:ext cx="695654" cy="1168823"/>
+          <a:off x="2409347" y="2293540"/>
+          <a:ext cx="986523" cy="1656306"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -352,15 +370,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>513844</xdr:colOff>
+      <xdr:colOff>356475</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>78027</xdr:rowOff>
+      <xdr:rowOff>28332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1344706</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>384036</xdr:rowOff>
+      <xdr:colOff>1532283</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>420696</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -389,8 +407,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8638109" y="750380"/>
-          <a:ext cx="830862" cy="1695538"/>
+          <a:off x="8498279" y="690941"/>
+          <a:ext cx="1175808" cy="2355342"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -401,23 +419,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>512802</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>139134</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257401</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1352085</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>90156</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1209261</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>325633</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagem 10">
+        <xdr:cNvPr id="13" name="Imagem 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC366CA7-2EEA-8195-8F53-D642EB502DDE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E053EFDE-4AA4-48B5-7891-00A507C5D8D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -425,7 +443,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -433,14 +451,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="16274"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8648546" y="2634219"/>
-          <a:ext cx="839283" cy="1651583"/>
+          <a:off x="2419162" y="680342"/>
+          <a:ext cx="951860" cy="1591704"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -452,22 +469,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>431336</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>75713</xdr:rowOff>
+      <xdr:colOff>181969</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76632</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1129199</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>223922</xdr:rowOff>
+      <xdr:colOff>1308652</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>401012</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagem 12">
+        <xdr:cNvPr id="19" name="Imagem 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E053EFDE-4AA4-48B5-7891-00A507C5D8D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F716A0CA-8F03-F680-3719-40BFCEDB4291}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -483,13 +500,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="16274"/>
+        <a:srcRect b="15452"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2657178" y="747476"/>
-          <a:ext cx="697863" cy="1180920"/>
+          <a:off x="2343730" y="10065458"/>
+          <a:ext cx="1126683" cy="1922924"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -501,22 +518,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>364187</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>159457</xdr:rowOff>
+      <xdr:colOff>164227</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>136084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1159017</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>348156</xdr:rowOff>
+      <xdr:colOff>1350064</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>573696</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagem 18">
+        <xdr:cNvPr id="21" name="Imagem 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F716A0CA-8F03-F680-3719-40BFCEDB4291}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4DE866A-7128-9D6C-B2AC-CA5FA7C2CA60}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -532,13 +549,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="15452"/>
+        <a:srcRect b="18475"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2525377" y="8429785"/>
-          <a:ext cx="794830" cy="1357974"/>
+          <a:off x="2325988" y="12311519"/>
+          <a:ext cx="1185837" cy="1945047"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -550,22 +567,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>338163</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>367997</xdr:rowOff>
+      <xdr:colOff>122402</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>182087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1234109</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>330121</xdr:rowOff>
+      <xdr:colOff>1350065</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>87357</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Imagem 20">
+        <xdr:cNvPr id="23" name="Imagem 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4DE866A-7128-9D6C-B2AC-CA5FA7C2CA60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBA9759-19DF-0FD2-F621-77A4F1FA4B1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -581,13 +598,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="18475"/>
+        <a:srcRect b="16686"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2499924" y="10381671"/>
-          <a:ext cx="895946" cy="1469559"/>
+          <a:off x="2284163" y="14701500"/>
+          <a:ext cx="1227663" cy="2050466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -599,22 +616,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>279772</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>223501</xdr:rowOff>
+      <xdr:colOff>123945</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>77443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1225825</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>39421</xdr:rowOff>
+      <xdr:colOff>1366631</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>733866</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Imagem 22">
+        <xdr:cNvPr id="27" name="Imagem 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBA9759-19DF-0FD2-F621-77A4F1FA4B1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B27889-D50D-B3D5-3D25-7332A2BC72F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -630,13 +647,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="16686"/>
+        <a:srcRect b="17209"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2441533" y="12581153"/>
-          <a:ext cx="946053" cy="1580116"/>
+          <a:off x="2285706" y="20063378"/>
+          <a:ext cx="1242686" cy="2072749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -648,22 +665,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>331010</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>135422</xdr:rowOff>
+      <xdr:colOff>192492</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>98641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1196995</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>751588</xdr:rowOff>
+      <xdr:colOff>1283804</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>332461</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Imagem 26">
+        <xdr:cNvPr id="31" name="Imagem 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B27889-D50D-B3D5-3D25-7332A2BC72F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1F8664-2D4F-5A32-8A34-742623342B9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -679,13 +696,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="17209"/>
+        <a:srcRect b="17246"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2492452" y="15316807"/>
-          <a:ext cx="865985" cy="1447193"/>
+          <a:off x="2354253" y="8066511"/>
+          <a:ext cx="1091312" cy="1824080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -697,22 +714,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>366427</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>156620</xdr:rowOff>
+      <xdr:colOff>218775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132009</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1123293</xdr:colOff>
+      <xdr:colOff>1300369</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>212428</xdr:rowOff>
+      <xdr:rowOff>257603</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Imagem 30">
+        <xdr:cNvPr id="33" name="Imagem 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1F8664-2D4F-5A32-8A34-742623342B9E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9241916E-320C-1CEA-B1FB-8D314EC20B9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -728,13 +745,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="17246"/>
+        <a:srcRect b="17582"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2527617" y="6791275"/>
-          <a:ext cx="756866" cy="1264498"/>
+          <a:off x="2380536" y="6045792"/>
+          <a:ext cx="1081594" cy="1798681"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -746,22 +763,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>367863</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>140292</xdr:rowOff>
+      <xdr:colOff>242469</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>113158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1128631</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>154768</xdr:rowOff>
+      <xdr:colOff>1242391</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>289924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Imagem 32">
+        <xdr:cNvPr id="35" name="Imagem 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9241916E-320C-1CEA-B1FB-8D314EC20B9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1388CE95-8672-C118-DA7F-891E04BEA808}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -777,13 +794,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="17582"/>
+        <a:srcRect b="17391"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2529053" y="5145844"/>
-          <a:ext cx="760768" cy="1262579"/>
+          <a:off x="2404230" y="4097093"/>
+          <a:ext cx="999922" cy="1684201"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -795,22 +812,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>424686</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>113158</xdr:rowOff>
+      <xdr:colOff>81893</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>221972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1122549</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>104178</xdr:rowOff>
+      <xdr:colOff>1385548</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>231912</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Imagem 34">
+        <xdr:cNvPr id="37" name="Imagem 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1388CE95-8672-C118-DA7F-891E04BEA808}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A01B941-02A6-98E0-295F-51049610827E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -826,62 +843,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="17391"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2585129" y="3511851"/>
-          <a:ext cx="697863" cy="1168657"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>288960</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>362777</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1226870</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>149086</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Imagem 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A01B941-02A6-98E0-295F-51049610827E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
         <a:srcRect b="17039"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2450721" y="15072690"/>
-          <a:ext cx="937910" cy="1550505"/>
+          <a:off x="2243654" y="17474646"/>
+          <a:ext cx="1303655" cy="2155136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1190,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
-  <dimension ref="B1:H38"/>
+  <dimension ref="B1:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,354 +1196,405 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="14"/>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+      <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15"/>
+      <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15"/>
+      <c r="C29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="16"/>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="C31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="11"/>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="12"/>
+      <c r="C33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="11"/>
+      <c r="C35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="11"/>
+      <c r="C36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="11"/>
+      <c r="C37" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="9" t="s">
+      <c r="D37" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
-      <c r="C34" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
+      <c r="C38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="10"/>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="11"/>
+      <c r="C40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="11"/>
+      <c r="C41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="11"/>
+      <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="12"/>
+      <c r="C43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="10"/>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="11"/>
+      <c r="C45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="12"/>
+      <c r="C46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="G8:G12"/>
-    <mergeCell ref="H8:H12"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
+  <mergeCells count="19">
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="F3:F9"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remoção do microfrontend Statistics Alterou: diagrama, task 3 e Stats markdown
</commit_message>
<xml_diff>
--- a/front-end/Task 3.xlsx
+++ b/front-end/Task 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7968ADE4-81EF-4F56-BFF9-429A184DCC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6519C3C-F54D-4AD0-A645-ADB03B0A27B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Views</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>Stats</t>
   </si>
   <si>
     <t>Move Positive</t>
@@ -266,14 +263,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,17 +281,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1161,7 +1158,7 @@
   <dimension ref="B1:H47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,91 +1194,91 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="D6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>20</v>
+      <c r="B7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1290,282 +1287,282 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="4" t="s">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+      <c r="C21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
     </row>
     <row r="27" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="13"/>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="C31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="11"/>
+      <c r="C33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+      <c r="C36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+      <c r="C37" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="11"/>
+      <c r="C38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="12"/>
-      <c r="C38" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="10"/>
+      <c r="C41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="10"/>
+      <c r="C42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11"/>
+      <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
-      <c r="C43" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="10"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="11"/>
+      <c r="C46" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="12"/>
-      <c r="C46" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D46" s="4"/>
     </row>
@@ -1576,6 +1573,10 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H9"/>
     <mergeCell ref="B39:B43"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="F3:F9"/>
@@ -1591,10 +1592,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H7:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert task 3 para ter Stats na viewmodel
</commit_message>
<xml_diff>
--- a/front-end/Task 3.xlsx
+++ b/front-end/Task 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6519C3C-F54D-4AD0-A645-ADB03B0A27B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAB2588-7731-4490-8038-CCE2CD7277B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Views</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Top Bar + Header</t>
+  </si>
+  <si>
+    <t>Stats</t>
   </si>
 </sst>
 </file>
@@ -269,6 +272,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,15 +298,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1157,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
   <dimension ref="B1:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,91 +1197,91 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="12"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="15" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="15" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1287,134 +1290,134 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="15" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
     </row>
     <row r="27" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2" t="s">
         <v>13</v>
       </c>
@@ -1423,7 +1426,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1435,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1441,21 +1444,21 @@
       </c>
     </row>
     <row r="31" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="2" t="s">
         <v>18</v>
       </c>
@@ -1464,14 +1467,14 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="2" t="s">
         <v>31</v>
       </c>
@@ -1480,7 +1483,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1489,7 +1492,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="2" t="s">
         <v>20</v>
       </c>
@@ -1498,21 +1501,21 @@
       </c>
     </row>
     <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="2" t="s">
         <v>15</v>
       </c>
@@ -1521,14 +1524,14 @@
       </c>
     </row>
     <row r="41" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="2" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1540,7 @@
       </c>
     </row>
     <row r="43" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
@@ -1546,21 +1549,21 @@
       </c>
     </row>
     <row r="44" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="4" t="s">
         <v>26</v>
       </c>
@@ -1573,11 +1576,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="B39:B43"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="F3:F9"/>
     <mergeCell ref="B17:B21"/>
@@ -1592,6 +1590,11 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="B39:B43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
alterações feitas de modo a ficarem mais corretas
</commit_message>
<xml_diff>
--- a/front-end/Task 3.xlsx
+++ b/front-end/Task 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F447F1C-91AD-48A4-B9BD-546F58F00E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3D9633-FEBA-47C4-837D-845D83A5F7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>Views</t>
   </si>
@@ -171,18 +171,12 @@
     <t>Meat.moreInfo</t>
   </si>
   <si>
-    <t>Meat.generalInfo</t>
-  </si>
-  <si>
     <t>Market.highlights</t>
   </si>
   <si>
     <t>Market.allMeats</t>
   </si>
   <si>
-    <t>Meat.info</t>
-  </si>
-  <si>
     <t>Profile photo</t>
   </si>
   <si>
@@ -196,6 +190,9 @@
   </si>
   <si>
     <t>Main.highlights</t>
+  </si>
+  <si>
+    <t>Meat.details</t>
   </si>
 </sst>
 </file>
@@ -323,6 +320,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -340,15 +346,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1211,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
   <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,131 +1245,129 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="12"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="15" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>51</v>
+      <c r="H4" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="15" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+        <v>51</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+        <v>52</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1376,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
@@ -1390,7 +1385,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1399,21 +1394,21 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1422,7 +1417,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1431,7 +1426,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1440,45 +1435,45 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="15" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1487,7 +1482,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1491,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="2" t="s">
         <v>13</v>
       </c>
@@ -1505,39 +1500,39 @@
       </c>
     </row>
     <row r="32" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="2" t="s">
         <v>27</v>
       </c>
@@ -1546,39 +1541,37 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="2" t="s">
         <v>14</v>
       </c>
@@ -1587,46 +1580,46 @@
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="4" t="s">
         <v>22</v>
       </c>
@@ -1639,11 +1632,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="B40:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="F3:F10"/>
     <mergeCell ref="B18:B22"/>
@@ -1658,6 +1646,11 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="B8:B12"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="B40:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Foto final do FE_blueprint e alterações na task3 de modo a ter o feedback
</commit_message>
<xml_diff>
--- a/front-end/Task 3.xlsx
+++ b/front-end/Task 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3D9633-FEBA-47C4-837D-845D83A5F7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD8A08E-90D0-4603-ABE8-32A6B57E5805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Views</t>
   </si>
@@ -193,6 +193,36 @@
   </si>
   <si>
     <t>Meat.details</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>Cancel button</t>
+  </si>
+  <si>
+    <t>Confirm button</t>
+  </si>
+  <si>
+    <t>Meat.starts</t>
+  </si>
+  <si>
+    <t>Meat Info</t>
+  </si>
+  <si>
+    <t>Ratings</t>
+  </si>
+  <si>
+    <t>Save Product Button</t>
+  </si>
+  <si>
+    <t>Give Feedback Button</t>
+  </si>
+  <si>
+    <t>Meat.smallInfo</t>
+  </si>
+  <si>
+    <t>Meat.feedbackUsers</t>
   </si>
 </sst>
 </file>
@@ -294,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,15 +350,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,6 +367,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,15 +451,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>356475</xdr:colOff>
+      <xdr:colOff>339157</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28332</xdr:rowOff>
+      <xdr:rowOff>201514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1532283</xdr:colOff>
+      <xdr:colOff>1514965</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>80517</xdr:rowOff>
+      <xdr:rowOff>253699</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -455,8 +488,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8498279" y="690941"/>
-          <a:ext cx="1175808" cy="2355342"/>
+          <a:off x="8478702" y="859605"/>
+          <a:ext cx="1175808" cy="2390139"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -902,6 +935,126 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>591286</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>21027</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>120350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>367392</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FFD7763-9901-9C64-182E-32D2704FFF4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8116036" y="6729348"/>
+          <a:ext cx="1964743" cy="1611830"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>320590</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>223158</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1578428</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>339998</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A886F0B7-37C1-1121-7839-1A5BC2300F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="13237" t="7979" r="16309" b="22864"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8457661" y="3665765"/>
+          <a:ext cx="1257838" cy="2157912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1208,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
   <dimension ref="B1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,235 +1398,298 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="15"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="15"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="9" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="4"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="4"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="4"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
       <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
       <c r="C20" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
       <c r="C21" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
       <c r="C22" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
       <c r="C23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16"/>
-      <c r="C24" s="9" t="s">
+      <c r="F23" s="14"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="17"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
+    <row r="25" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12"/>
       <c r="C28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="16"/>
+    <row r="29" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="13"/>
       <c r="C29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1481,8 +1697,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
+    <row r="30" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="13"/>
       <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1490,8 +1706,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="17"/>
+    <row r="31" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
       <c r="C31" s="2" t="s">
         <v>13</v>
       </c>
@@ -1499,15 +1715,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
+    <row r="32" spans="2:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
       <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="2" t="s">
         <v>15</v>
       </c>
@@ -1516,7 +1732,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="14"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="2" t="s">
         <v>16</v>
       </c>
@@ -1525,14 +1741,14 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="13"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="2" t="s">
         <v>27</v>
       </c>
@@ -1541,7 +1757,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="13"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="2" t="s">
         <v>28</v>
       </c>
@@ -1550,28 +1766,28 @@
       </c>
     </row>
     <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="13"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="14"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="2" t="s">
         <v>14</v>
       </c>
@@ -1580,14 +1796,14 @@
       </c>
     </row>
     <row r="42" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="2" t="s">
         <v>16</v>
       </c>
@@ -1596,7 +1812,7 @@
       </c>
     </row>
     <row r="44" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="14"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="2" t="s">
         <v>19</v>
       </c>
@@ -1605,21 +1821,21 @@
       </c>
     </row>
     <row r="45" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="12"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="13"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="14"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="4" t="s">
         <v>22</v>
       </c>
@@ -1631,7 +1847,23 @@
       <c r="D48" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="31">
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="F11:F17"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="F3:F10"/>
     <mergeCell ref="B18:B22"/>
@@ -1646,11 +1878,7 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="B8:B12"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="F18:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>